<commit_message>
Manipal data on sheet 2.
</commit_message>
<xml_diff>
--- a/DataIIT1004.xlsx
+++ b/DataIIT1004.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$J$935</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4864" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5028" uniqueCount="347">
   <si>
     <t>Name of Insti</t>
   </si>
@@ -985,13 +986,97 @@
   </si>
   <si>
     <t>BITS Goa</t>
+  </si>
+  <si>
+    <t>Aeronautical Engineering      </t>
+  </si>
+  <si>
+    <t>Automobile Engineering       </t>
+  </si>
+  <si>
+    <t>Biochemical Engineering      </t>
+  </si>
+  <si>
+    <t>Biotechnology Engineering   </t>
+  </si>
+  <si>
+    <t>Chemical Engineering</t>
+  </si>
+  <si>
+    <t>Civil Engineering      </t>
+  </si>
+  <si>
+    <t>Electronics and Computer Engineering         </t>
+  </si>
+  <si>
+    <t>Computer Science Engineering         </t>
+  </si>
+  <si>
+    <t>Electrical and Electronics Engineering          </t>
+  </si>
+  <si>
+    <t>Electronics and Communication Engineering</t>
+  </si>
+  <si>
+    <t>Instrumentation and Control Engineering      </t>
+  </si>
+  <si>
+    <t>Industrial and Production Engineering          </t>
+  </si>
+  <si>
+    <t>Information Technology        </t>
+  </si>
+  <si>
+    <t>Mechanical Engineering        </t>
+  </si>
+  <si>
+    <t>Mechatronics Engineering     </t>
+  </si>
+  <si>
+    <t>Printing Technology  </t>
+  </si>
+  <si>
+    <t>MUOET</t>
+  </si>
+  <si>
+    <t>Manipal University, Manipal</t>
+  </si>
+  <si>
+    <t>Manipal Institute of Technology, Sikkim</t>
+  </si>
+  <si>
+    <t>Manipal University, Jaipur</t>
+  </si>
+  <si>
+    <t>BITS Hyderabad</t>
+  </si>
+  <si>
+    <t>Information Technology</t>
+  </si>
+  <si>
+    <t>Mechanical Engineering</t>
+  </si>
+  <si>
+    <t>Mechatronics Engineering</t>
+  </si>
+  <si>
+    <t>Computer Science Engineering</t>
+  </si>
+  <si>
+    <t>Electronics and Computer Engineering</t>
+  </si>
+  <si>
+    <t>Civil Engineering</t>
+  </si>
+  <si>
+    <t>Automobile Engineering</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1009,6 +1094,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF111111"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1032,7 +1123,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1120,11 +1211,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFE6E5E5"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFE6E5E5"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFE6E5E5"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFE6E5E5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFE6E5E5"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFE6E5E5"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1144,6 +1261,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1155,6 +1273,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1506,8 +1633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AMK974"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A963" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J973" sqref="J973"/>
+    <sheetView topLeftCell="A963" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B954" sqref="B954"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -28608,13 +28735,13 @@
       <c r="B936" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C936" s="7" t="s">
+      <c r="C936" s="8" t="s">
         <v>300</v>
       </c>
       <c r="D936" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F936" s="8">
+      <c r="F936" s="9">
         <v>306</v>
       </c>
       <c r="G936" s="1" t="s">
@@ -28634,13 +28761,13 @@
       <c r="B937" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C937" s="7" t="s">
+      <c r="C937" s="8" t="s">
         <v>301</v>
       </c>
       <c r="D937" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F937" s="8">
+      <c r="F937" s="9">
         <v>294</v>
       </c>
       <c r="G937" s="1" t="s">
@@ -28660,13 +28787,13 @@
       <c r="B938" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C938" s="7" t="s">
+      <c r="C938" s="8" t="s">
         <v>302</v>
       </c>
       <c r="D938" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F938" s="8">
+      <c r="F938" s="9">
         <v>355</v>
       </c>
       <c r="G938" s="1" t="s">
@@ -28686,13 +28813,13 @@
       <c r="B939" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C939" s="7" t="s">
+      <c r="C939" s="8" t="s">
         <v>303</v>
       </c>
       <c r="D939" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F939" s="8">
+      <c r="F939" s="9">
         <v>334</v>
       </c>
       <c r="G939" s="1" t="s">
@@ -28712,13 +28839,13 @@
       <c r="B940" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C940" s="7" t="s">
+      <c r="C940" s="8" t="s">
         <v>304</v>
       </c>
       <c r="D940" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F940" s="8">
+      <c r="F940" s="9">
         <v>288</v>
       </c>
       <c r="G940" s="1" t="s">
@@ -28738,13 +28865,13 @@
       <c r="B941" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C941" s="7" t="s">
+      <c r="C941" s="8" t="s">
         <v>305</v>
       </c>
       <c r="D941" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F941" s="8">
+      <c r="F941" s="9">
         <v>221</v>
       </c>
       <c r="G941" s="1" t="s">
@@ -28764,13 +28891,13 @@
       <c r="B942" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C942" s="7" t="s">
+      <c r="C942" s="8" t="s">
         <v>306</v>
       </c>
       <c r="D942" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F942" s="8">
+      <c r="F942" s="9">
         <v>382</v>
       </c>
       <c r="G942" s="1" t="s">
@@ -28790,13 +28917,13 @@
       <c r="B943" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C943" s="7" t="s">
+      <c r="C943" s="8" t="s">
         <v>307</v>
       </c>
       <c r="D943" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F943" s="8">
+      <c r="F943" s="9">
         <v>332</v>
       </c>
       <c r="G943" s="1" t="s">
@@ -28816,13 +28943,13 @@
       <c r="B944" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C944" s="7" t="s">
+      <c r="C944" s="8" t="s">
         <v>308</v>
       </c>
       <c r="D944" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F944" s="8">
+      <c r="F944" s="9">
         <v>237</v>
       </c>
       <c r="G944" s="1" t="s">
@@ -28842,13 +28969,13 @@
       <c r="B945" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C945" s="7" t="s">
+      <c r="C945" s="8" t="s">
         <v>309</v>
       </c>
       <c r="D945" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F945" s="8">
+      <c r="F945" s="9">
         <v>265</v>
       </c>
       <c r="G945" s="1" t="s">
@@ -28868,13 +28995,13 @@
       <c r="B946" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C946" s="7" t="s">
+      <c r="C946" s="8" t="s">
         <v>310</v>
       </c>
       <c r="D946" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F946" s="8">
+      <c r="F946" s="9">
         <v>323</v>
       </c>
       <c r="G946" s="1" t="s">
@@ -28894,13 +29021,13 @@
       <c r="B947" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C947" s="7" t="s">
+      <c r="C947" s="8" t="s">
         <v>311</v>
       </c>
       <c r="D947" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F947" s="8">
+      <c r="F947" s="9">
         <v>312</v>
       </c>
       <c r="G947" s="1" t="s">
@@ -28920,13 +29047,13 @@
       <c r="B948" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C948" s="9" t="s">
+      <c r="C948" s="10" t="s">
         <v>312</v>
       </c>
       <c r="D948" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F948" s="10">
+      <c r="F948" s="11">
         <v>304</v>
       </c>
       <c r="G948" s="1" t="s">
@@ -28946,13 +29073,13 @@
       <c r="B949" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="C949" s="7" t="s">
+      <c r="C949" s="8" t="s">
         <v>300</v>
       </c>
       <c r="D949" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F949" s="8">
+      <c r="F949" s="9">
         <v>276</v>
       </c>
       <c r="G949" s="1" t="s">
@@ -28972,13 +29099,13 @@
       <c r="B950" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="C950" s="7" t="s">
+      <c r="C950" s="8" t="s">
         <v>316</v>
       </c>
       <c r="D950" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F950" s="8">
+      <c r="F950" s="9">
         <v>320</v>
       </c>
       <c r="G950" s="1" t="s">
@@ -28998,13 +29125,13 @@
       <c r="B951" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="C951" s="7" t="s">
+      <c r="C951" s="8" t="s">
         <v>303</v>
       </c>
       <c r="D951" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F951" s="8">
+      <c r="F951" s="9">
         <v>304</v>
       </c>
       <c r="G951" s="1" t="s">
@@ -29024,13 +29151,13 @@
       <c r="B952" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="C952" s="7" t="s">
+      <c r="C952" s="8" t="s">
         <v>306</v>
       </c>
       <c r="D952" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F952" s="8">
+      <c r="F952" s="9">
         <v>350</v>
       </c>
       <c r="G952" s="1" t="s">
@@ -29050,13 +29177,13 @@
       <c r="B953" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="C953" s="7" t="s">
+      <c r="C953" s="8" t="s">
         <v>307</v>
       </c>
       <c r="D953" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F953" s="8">
+      <c r="F953" s="9">
         <v>301</v>
       </c>
       <c r="G953" s="1" t="s">
@@ -29076,13 +29203,13 @@
       <c r="B954" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="C954" s="7" t="s">
+      <c r="C954" s="8" t="s">
         <v>317</v>
       </c>
       <c r="D954" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F954" s="8">
+      <c r="F954" s="9">
         <v>322</v>
       </c>
       <c r="G954" s="1" t="s">
@@ -29102,13 +29229,13 @@
       <c r="B955" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="C955" s="7" t="s">
+      <c r="C955" s="8" t="s">
         <v>308</v>
       </c>
       <c r="D955" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F955" s="8">
+      <c r="F955" s="9">
         <v>202</v>
       </c>
       <c r="G955" s="1" t="s">
@@ -29128,13 +29255,13 @@
       <c r="B956" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="C956" s="7" t="s">
+      <c r="C956" s="8" t="s">
         <v>309</v>
       </c>
       <c r="D956" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F956" s="8">
+      <c r="F956" s="9">
         <v>235</v>
       </c>
       <c r="G956" s="1" t="s">
@@ -29154,13 +29281,13 @@
       <c r="B957" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="C957" s="7" t="s">
+      <c r="C957" s="8" t="s">
         <v>310</v>
       </c>
       <c r="D957" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F957" s="8">
+      <c r="F957" s="9">
         <v>290</v>
       </c>
       <c r="G957" s="1" t="s">
@@ -29180,13 +29307,13 @@
       <c r="B958" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="C958" s="7" t="s">
+      <c r="C958" s="8" t="s">
         <v>311</v>
       </c>
       <c r="D958" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F958" s="8">
+      <c r="F958" s="9">
         <v>273</v>
       </c>
       <c r="G958" s="1" t="s">
@@ -29206,13 +29333,13 @@
       <c r="B959" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="C959" s="9" t="s">
+      <c r="C959" s="10" t="s">
         <v>312</v>
       </c>
       <c r="D959" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F959" s="10">
+      <c r="F959" s="11">
         <v>270</v>
       </c>
       <c r="G959" s="1" t="s">
@@ -29230,15 +29357,15 @@
     </row>
     <row r="960" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="B960" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C960" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C960" s="8" t="s">
         <v>300</v>
       </c>
       <c r="D960" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F960" s="8">
+      <c r="F960" s="9">
         <v>272</v>
       </c>
       <c r="G960" s="1" t="s">
@@ -29256,15 +29383,15 @@
     </row>
     <row r="961" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="B961" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C961" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C961" s="8" t="s">
         <v>301</v>
       </c>
       <c r="D961" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F961" s="8">
+      <c r="F961" s="9">
         <v>273</v>
       </c>
       <c r="G961" s="1" t="s">
@@ -29282,15 +29409,15 @@
     </row>
     <row r="962" spans="2:10" ht="39.75" thickTop="1" thickBot="1">
       <c r="B962" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C962" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C962" s="8" t="s">
         <v>316</v>
       </c>
       <c r="D962" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F962" s="8">
+      <c r="F962" s="9">
         <v>310</v>
       </c>
       <c r="G962" s="1" t="s">
@@ -29308,15 +29435,15 @@
     </row>
     <row r="963" spans="2:10" ht="27" thickTop="1" thickBot="1">
       <c r="B963" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C963" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C963" s="8" t="s">
         <v>303</v>
       </c>
       <c r="D963" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F963" s="8">
+      <c r="F963" s="9">
         <v>297</v>
       </c>
       <c r="G963" s="1" t="s">
@@ -29334,15 +29461,15 @@
     </row>
     <row r="964" spans="2:10" ht="27" thickTop="1" thickBot="1">
       <c r="B964" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C964" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C964" s="8" t="s">
         <v>306</v>
       </c>
       <c r="D964" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F964" s="8">
+      <c r="F964" s="9">
         <v>339</v>
       </c>
       <c r="G964" s="1" t="s">
@@ -29360,15 +29487,15 @@
     </row>
     <row r="965" spans="2:10" ht="39.75" thickTop="1" thickBot="1">
       <c r="B965" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C965" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C965" s="8" t="s">
         <v>317</v>
       </c>
       <c r="D965" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F965" s="8">
+      <c r="F965" s="9">
         <v>320</v>
       </c>
       <c r="G965" s="1" t="s">
@@ -29386,15 +29513,15 @@
     </row>
     <row r="966" spans="2:10" ht="52.5" thickTop="1" thickBot="1">
       <c r="B966" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C966" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C966" s="8" t="s">
         <v>307</v>
       </c>
       <c r="D966" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F966" s="8">
+      <c r="F966" s="9">
         <v>298</v>
       </c>
       <c r="G966" s="1" t="s">
@@ -29412,15 +29539,15 @@
     </row>
     <row r="967" spans="2:10" ht="27" thickTop="1" thickBot="1">
       <c r="B967" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C967" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C967" s="8" t="s">
         <v>304</v>
       </c>
       <c r="D967" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F967" s="8">
+      <c r="F967" s="9">
         <v>269</v>
       </c>
       <c r="G967" s="1" t="s">
@@ -29438,15 +29565,15 @@
     </row>
     <row r="968" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="B968" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C968" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C968" s="8" t="s">
         <v>305</v>
       </c>
       <c r="D968" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F968" s="8">
+      <c r="F968" s="9">
         <v>200</v>
       </c>
       <c r="G968" s="1" t="s">
@@ -29464,15 +29591,15 @@
     </row>
     <row r="969" spans="2:10" ht="39.75" thickTop="1" thickBot="1">
       <c r="B969" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C969" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C969" s="8" t="s">
         <v>308</v>
       </c>
       <c r="D969" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F969" s="8">
+      <c r="F969" s="9">
         <v>202</v>
       </c>
       <c r="G969" s="1" t="s">
@@ -29490,15 +29617,15 @@
     </row>
     <row r="970" spans="2:10" ht="27" thickTop="1" thickBot="1">
       <c r="B970" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C970" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C970" s="8" t="s">
         <v>309</v>
       </c>
       <c r="D970" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F970" s="8">
+      <c r="F970" s="9">
         <v>222</v>
       </c>
       <c r="G970" s="1" t="s">
@@ -29516,15 +29643,15 @@
     </row>
     <row r="971" spans="2:10" ht="27" thickTop="1" thickBot="1">
       <c r="B971" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C971" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C971" s="8" t="s">
         <v>310</v>
       </c>
       <c r="D971" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F971" s="8">
+      <c r="F971" s="9">
         <v>279</v>
       </c>
       <c r="G971" s="1" t="s">
@@ -29542,15 +29669,15 @@
     </row>
     <row r="972" spans="2:10" ht="27" thickTop="1" thickBot="1">
       <c r="B972" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C972" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C972" s="8" t="s">
         <v>311</v>
       </c>
       <c r="D972" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F972" s="8">
+      <c r="F972" s="9">
         <v>258</v>
       </c>
       <c r="G972" s="1" t="s">
@@ -29568,15 +29695,15 @@
     </row>
     <row r="973" spans="2:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="B973" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C973" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="C973" s="10" t="s">
         <v>312</v>
       </c>
       <c r="D973" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F973" s="10">
+      <c r="F973" s="11">
         <v>251</v>
       </c>
       <c r="G973" s="1" t="s">
@@ -29598,4 +29725,858 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:J33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="42.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="12">
+        <v>11442</v>
+      </c>
+      <c r="G3" t="s">
+        <v>335</v>
+      </c>
+      <c r="H3">
+        <v>2017</v>
+      </c>
+      <c r="I3" t="s">
+        <v>315</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B4" t="s">
+        <v>336</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="12">
+        <v>10590</v>
+      </c>
+      <c r="G4" t="s">
+        <v>335</v>
+      </c>
+      <c r="H4">
+        <v>2017</v>
+      </c>
+      <c r="I4" t="s">
+        <v>315</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B5" t="s">
+        <v>336</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>321</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="12">
+        <v>36418</v>
+      </c>
+      <c r="G5" t="s">
+        <v>335</v>
+      </c>
+      <c r="H5">
+        <v>2017</v>
+      </c>
+      <c r="I5" t="s">
+        <v>315</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B6" t="s">
+        <v>336</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>322</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="12">
+        <v>24612</v>
+      </c>
+      <c r="G6" t="s">
+        <v>335</v>
+      </c>
+      <c r="H6">
+        <v>2017</v>
+      </c>
+      <c r="I6" t="s">
+        <v>315</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B7" t="s">
+        <v>336</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="12">
+        <v>11228</v>
+      </c>
+      <c r="G7" t="s">
+        <v>335</v>
+      </c>
+      <c r="H7">
+        <v>2017</v>
+      </c>
+      <c r="I7" t="s">
+        <v>315</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B8" t="s">
+        <v>336</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="12">
+        <v>16826</v>
+      </c>
+      <c r="G8" t="s">
+        <v>335</v>
+      </c>
+      <c r="H8">
+        <v>2017</v>
+      </c>
+      <c r="I8" t="s">
+        <v>315</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B9" t="s">
+        <v>336</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="12">
+        <v>4820</v>
+      </c>
+      <c r="G9" t="s">
+        <v>335</v>
+      </c>
+      <c r="H9">
+        <v>2017</v>
+      </c>
+      <c r="I9" t="s">
+        <v>315</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B10" t="s">
+        <v>336</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="12">
+        <v>1893</v>
+      </c>
+      <c r="G10" t="s">
+        <v>335</v>
+      </c>
+      <c r="H10">
+        <v>2017</v>
+      </c>
+      <c r="I10" t="s">
+        <v>315</v>
+      </c>
+      <c r="J10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B11" t="s">
+        <v>336</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="12">
+        <v>7433</v>
+      </c>
+      <c r="G11" t="s">
+        <v>335</v>
+      </c>
+      <c r="H11">
+        <v>2017</v>
+      </c>
+      <c r="I11" t="s">
+        <v>315</v>
+      </c>
+      <c r="J11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B12" t="s">
+        <v>336</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>328</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="12">
+        <v>4954</v>
+      </c>
+      <c r="G12" t="s">
+        <v>335</v>
+      </c>
+      <c r="H12">
+        <v>2017</v>
+      </c>
+      <c r="I12" t="s">
+        <v>315</v>
+      </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B13" t="s">
+        <v>336</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="12">
+        <v>18405</v>
+      </c>
+      <c r="G13" t="s">
+        <v>335</v>
+      </c>
+      <c r="H13">
+        <v>2017</v>
+      </c>
+      <c r="I13" t="s">
+        <v>315</v>
+      </c>
+      <c r="J13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B14" t="s">
+        <v>336</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="12">
+        <v>16236</v>
+      </c>
+      <c r="G14" t="s">
+        <v>335</v>
+      </c>
+      <c r="H14">
+        <v>2017</v>
+      </c>
+      <c r="I14" t="s">
+        <v>315</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B15" t="s">
+        <v>336</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="12">
+        <v>3244</v>
+      </c>
+      <c r="G15" t="s">
+        <v>335</v>
+      </c>
+      <c r="H15">
+        <v>2017</v>
+      </c>
+      <c r="I15" t="s">
+        <v>315</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B16" t="s">
+        <v>336</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="12">
+        <v>6138</v>
+      </c>
+      <c r="G16" t="s">
+        <v>335</v>
+      </c>
+      <c r="H16">
+        <v>2017</v>
+      </c>
+      <c r="I16" t="s">
+        <v>315</v>
+      </c>
+      <c r="J16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B17" t="s">
+        <v>336</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="12">
+        <v>8218</v>
+      </c>
+      <c r="G17" t="s">
+        <v>335</v>
+      </c>
+      <c r="H17">
+        <v>2017</v>
+      </c>
+      <c r="I17" t="s">
+        <v>315</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B18" t="s">
+        <v>336</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="12">
+        <v>40454</v>
+      </c>
+      <c r="G18" t="s">
+        <v>335</v>
+      </c>
+      <c r="H18">
+        <v>2017</v>
+      </c>
+      <c r="I18" t="s">
+        <v>315</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B19" t="s">
+        <v>337</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="13">
+        <v>33258</v>
+      </c>
+      <c r="G19" t="s">
+        <v>335</v>
+      </c>
+      <c r="H19">
+        <v>2017</v>
+      </c>
+      <c r="I19" t="s">
+        <v>315</v>
+      </c>
+      <c r="J19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B20" t="s">
+        <v>337</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="12">
+        <v>41708</v>
+      </c>
+      <c r="G20" t="s">
+        <v>335</v>
+      </c>
+      <c r="H20">
+        <v>2017</v>
+      </c>
+      <c r="I20" t="s">
+        <v>315</v>
+      </c>
+      <c r="J20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B21" t="s">
+        <v>337</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="12">
+        <v>38681</v>
+      </c>
+      <c r="G21" t="s">
+        <v>335</v>
+      </c>
+      <c r="H21">
+        <v>2017</v>
+      </c>
+      <c r="I21" t="s">
+        <v>315</v>
+      </c>
+      <c r="J21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B22" t="s">
+        <v>337</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>328</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="12">
+        <v>39356</v>
+      </c>
+      <c r="G22" t="s">
+        <v>335</v>
+      </c>
+      <c r="H22">
+        <v>2017</v>
+      </c>
+      <c r="I22" t="s">
+        <v>315</v>
+      </c>
+      <c r="J22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B23" t="s">
+        <v>337</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="12">
+        <v>32120</v>
+      </c>
+      <c r="G23" t="s">
+        <v>335</v>
+      </c>
+      <c r="H23">
+        <v>2017</v>
+      </c>
+      <c r="I23" t="s">
+        <v>315</v>
+      </c>
+      <c r="J23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B24" t="s">
+        <v>337</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="12">
+        <v>38134</v>
+      </c>
+      <c r="G24" t="s">
+        <v>335</v>
+      </c>
+      <c r="H24">
+        <v>2017</v>
+      </c>
+      <c r="I24" t="s">
+        <v>315</v>
+      </c>
+      <c r="J24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B25" t="s">
+        <v>338</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="12">
+        <v>40312</v>
+      </c>
+      <c r="G25" t="s">
+        <v>335</v>
+      </c>
+      <c r="H25">
+        <v>2017</v>
+      </c>
+      <c r="I25" t="s">
+        <v>315</v>
+      </c>
+      <c r="J25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B26" t="s">
+        <v>338</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="12">
+        <v>36477</v>
+      </c>
+      <c r="G26" t="s">
+        <v>335</v>
+      </c>
+      <c r="H26">
+        <v>2017</v>
+      </c>
+      <c r="I26" t="s">
+        <v>315</v>
+      </c>
+      <c r="J26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B27" t="s">
+        <v>338</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>345</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="12">
+        <v>40807</v>
+      </c>
+      <c r="G27" t="s">
+        <v>335</v>
+      </c>
+      <c r="H27">
+        <v>2017</v>
+      </c>
+      <c r="I27" t="s">
+        <v>315</v>
+      </c>
+      <c r="J27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B28" t="s">
+        <v>338</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="12">
+        <v>25593</v>
+      </c>
+      <c r="G28" t="s">
+        <v>335</v>
+      </c>
+      <c r="H28">
+        <v>2017</v>
+      </c>
+      <c r="I28" t="s">
+        <v>315</v>
+      </c>
+      <c r="J28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B29" t="s">
+        <v>338</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="12">
+        <v>10867</v>
+      </c>
+      <c r="G29" t="s">
+        <v>335</v>
+      </c>
+      <c r="H29">
+        <v>2017</v>
+      </c>
+      <c r="I29" t="s">
+        <v>315</v>
+      </c>
+      <c r="J29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B30" t="s">
+        <v>338</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>328</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="12">
+        <v>24335</v>
+      </c>
+      <c r="G30" t="s">
+        <v>335</v>
+      </c>
+      <c r="H30">
+        <v>2017</v>
+      </c>
+      <c r="I30" t="s">
+        <v>315</v>
+      </c>
+      <c r="J30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B31" t="s">
+        <v>338</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="12">
+        <v>17195</v>
+      </c>
+      <c r="G31" t="s">
+        <v>335</v>
+      </c>
+      <c r="H31">
+        <v>2017</v>
+      </c>
+      <c r="I31" t="s">
+        <v>315</v>
+      </c>
+      <c r="J31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B32" t="s">
+        <v>338</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="12">
+        <v>28487</v>
+      </c>
+      <c r="G32" t="s">
+        <v>335</v>
+      </c>
+      <c r="H32">
+        <v>2017</v>
+      </c>
+      <c r="I32" t="s">
+        <v>315</v>
+      </c>
+      <c r="J32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" ht="15.75" thickBot="1">
+      <c r="B33" t="s">
+        <v>338</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>342</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="12">
+        <v>41629</v>
+      </c>
+      <c r="G33" t="s">
+        <v>335</v>
+      </c>
+      <c r="H33">
+        <v>2017</v>
+      </c>
+      <c r="I33" t="s">
+        <v>315</v>
+      </c>
+      <c r="J33">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>